<commit_message>
tăng độ chính xác khi truy vấn
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\AI\Project3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0815E5CA-9AE4-4080-8C57-87F18811FFF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B82F238A-3E8E-4D64-B336-2F3C08EC6C71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Quy trình chăm sóc khách hàng" sheetId="1" r:id="rId1"/>
     <sheet name="Tổng hợp thông tin dịch vụ" sheetId="2" r:id="rId2"/>
     <sheet name="Các câu hỏi thường gặp" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="176">
   <si>
     <t>Quy trình</t>
   </si>
@@ -233,12 +234,6 @@
   </si>
   <si>
     <t xml:space="preserve">Em gửi anh bộ report demo của sản phẩm ạ: https://docs.google.com/spreadsheets/d/1NQjDDoVGIj68j7YmVRDQu_Bj-8GNI8gu/edit?gid=443237055#gid=443237055 </t>
-  </si>
-  <si>
-    <t>Đây là video demo vận hành của phần mềm tạo entity ạ: https://www.youtube.com/watch?v=pxrUFSKvC10</t>
-  </si>
-  <si>
-    <t>Case study thực tế là kết quả của lần chạy demo nói trên ạ : https://scapbot.com/vi/likepion/</t>
   </si>
   <si>
     <t>Khai thác</t>
@@ -1640,6 +1635,96 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1667,45 +1752,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1720,57 +1766,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2055,8 +2050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2087,10 +2082,10 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="408.75" thickBot="1">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="44" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -2113,8 +2108,8 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="102.75" thickBot="1">
-      <c r="A3" s="12"/>
-      <c r="B3" s="15"/>
+      <c r="A3" s="42"/>
+      <c r="B3" s="45"/>
       <c r="C3" s="3" t="s">
         <v>11</v>
       </c>
@@ -2125,8 +2120,8 @@
       <c r="H3" s="3"/>
     </row>
     <row r="4" spans="1:8" ht="100.5" thickBot="1">
-      <c r="A4" s="12"/>
-      <c r="B4" s="14" t="s">
+      <c r="A4" s="42"/>
+      <c r="B4" s="44" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="6" t="s">
@@ -2138,24 +2133,20 @@
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:8" ht="72" thickBot="1">
-      <c r="A5" s="12"/>
-      <c r="B5" s="16"/>
-      <c r="C5" s="6" t="s">
-        <v>14</v>
-      </c>
+    <row r="5" spans="1:8" ht="15" thickBot="1">
+      <c r="A5" s="42"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="6"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:8" ht="72" thickBot="1">
-      <c r="A6" s="12"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="6" t="s">
-        <v>15</v>
-      </c>
+    <row r="6" spans="1:8" ht="15" thickBot="1">
+      <c r="A6" s="42"/>
+      <c r="B6" s="45"/>
+      <c r="C6" s="6"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
@@ -2163,43 +2154,43 @@
       <c r="H6" s="3"/>
     </row>
     <row r="7" spans="1:8" ht="408.75" thickBot="1">
-      <c r="A7" s="12"/>
-      <c r="B7" s="14" t="s">
+      <c r="A7" s="42"/>
+      <c r="B7" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="E7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="F7" s="5" t="s">
         <v>18</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>20</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8" ht="153.75" thickBot="1">
-      <c r="A8" s="12"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="19"/>
+      <c r="A8" s="42"/>
+      <c r="B8" s="46"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="49"/>
       <c r="E8" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:8" ht="15" thickBot="1">
-      <c r="A9" s="13"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="19"/>
+      <c r="A9" s="43"/>
+      <c r="B9" s="46"/>
+      <c r="C9" s="49"/>
       <c r="D9" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E9" s="7">
         <v>9</v>
@@ -2210,34 +2201,34 @@
     </row>
     <row r="10" spans="1:8" ht="408.75" thickBot="1">
       <c r="A10" s="3"/>
-      <c r="B10" s="16"/>
+      <c r="B10" s="46"/>
       <c r="C10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="F10" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="G10" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="H10" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="408.75" thickBot="1">
       <c r="A11" s="3"/>
-      <c r="B11" s="16"/>
+      <c r="B11" s="46"/>
       <c r="C11" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
@@ -2246,12 +2237,12 @@
     </row>
     <row r="12" spans="1:8" ht="357.75" thickBot="1">
       <c r="A12" s="3"/>
-      <c r="B12" s="16"/>
+      <c r="B12" s="46"/>
       <c r="C12" s="10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
@@ -2260,12 +2251,12 @@
     </row>
     <row r="13" spans="1:8" ht="179.25" thickBot="1">
       <c r="A13" s="3"/>
-      <c r="B13" s="15"/>
+      <c r="B13" s="45"/>
       <c r="C13" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
@@ -2274,17 +2265,15 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="D7:D8"/>
     <mergeCell ref="A2:A9"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="B4:B6"/>
     <mergeCell ref="B7:B13"/>
     <mergeCell ref="C7:C9"/>
-    <mergeCell ref="D7:D8"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C4" r:id="rId1" location="gid=443237055" display="https://docs.google.com/spreadsheets/d/1NQjDDoVGIj68j7YmVRDQu_Bj-8GNI8gu/edit?gid=443237055 - gid=443237055" xr:uid="{58BC9AC5-5CCB-45EE-9E84-AE434A1DA41E}"/>
-    <hyperlink ref="C5" r:id="rId2" display="https://www.youtube.com/watch?v=pxrUFSKvC10" xr:uid="{1EA1FFF6-7D89-40DF-8641-5AAAFFA2448D}"/>
-    <hyperlink ref="C6" r:id="rId3" display="https://scapbot.com/vi/likepion/" xr:uid="{4A98F2C6-6263-43C6-A17A-1031D0A27FE4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2294,8 +2283,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF7B9F1C-0209-470A-B394-69205212CDA4}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2308,192 +2297,192 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" thickBot="1">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>35</v>
-      </c>
-      <c r="B1" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" s="21" t="s">
-        <v>37</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="57.75" thickBot="1">
+      <c r="A2" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="14" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="57.75" thickBot="1">
-      <c r="A2" s="22" t="s">
+      <c r="C2" s="15"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="23" t="s">
+    </row>
+    <row r="3" spans="1:5" ht="399.75" thickBot="1">
+      <c r="A3" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="25" t="s">
+      <c r="B3" s="15" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="399.75" thickBot="1">
-      <c r="A3" s="26" t="s">
+      <c r="C3" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="D3" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="E3" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="3" t="s">
+    </row>
+    <row r="4" spans="1:5" ht="43.5" thickBot="1">
+      <c r="A4" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="B4" s="15"/>
+      <c r="C4" s="19" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="43.5" thickBot="1">
-      <c r="A4" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="28" t="s">
-        <v>48</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:5" ht="408.75" thickBot="1">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="D5" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="1:5" ht="86.25" thickBot="1">
+      <c r="A6" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="B6" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" spans="1:5" ht="86.25" thickBot="1">
-      <c r="A6" s="26" t="s">
+      <c r="C6" s="19" t="s">
         <v>53</v>
-      </c>
-      <c r="B6" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="C6" s="28" t="s">
-        <v>55</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:5" ht="100.5" thickBot="1">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="19" t="s">
         <v>56</v>
-      </c>
-      <c r="B7" s="28" t="s">
-        <v>57</v>
-      </c>
-      <c r="C7" s="28" t="s">
-        <v>58</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:5" ht="43.5" thickBot="1">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="19" t="s">
         <v>59</v>
-      </c>
-      <c r="B8" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="C8" s="28" t="s">
-        <v>61</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:5" ht="43.5" thickBot="1">
-      <c r="A9" s="32" t="s">
-        <v>62</v>
-      </c>
-      <c r="B9" s="33" t="s">
-        <v>63</v>
-      </c>
-      <c r="C9" s="34"/>
+      <c r="A9" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="50" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="51"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:5" ht="57.75" thickBot="1">
-      <c r="A10" s="32" t="s">
-        <v>64</v>
-      </c>
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
+      <c r="A10" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:5" ht="51.75" thickBot="1">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="52" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="15" t="s">
         <v>65</v>
-      </c>
-      <c r="B11" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="C11" s="24" t="s">
-        <v>67</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:5" ht="51.75" thickBot="1">
-      <c r="A12" s="36"/>
-      <c r="B12" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="C12" s="24" t="s">
-        <v>69</v>
+      <c r="A12" s="53"/>
+      <c r="B12" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>67</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:5" ht="15" thickBot="1">
-      <c r="A13" s="36"/>
-      <c r="B13" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="C13" s="24"/>
+      <c r="A13" s="53"/>
+      <c r="B13" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="15"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
     </row>
     <row r="14" spans="1:5" ht="15" thickBot="1">
-      <c r="A14" s="36"/>
-      <c r="B14" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="C14" s="24"/>
+      <c r="A14" s="53"/>
+      <c r="B14" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" s="15"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
     </row>
     <row r="15" spans="1:5" ht="26.25" thickBot="1">
-      <c r="A15" s="36"/>
-      <c r="B15" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="C15" s="24"/>
+      <c r="A15" s="53"/>
+      <c r="B15" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" s="15"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:5" ht="15" thickBot="1">
-      <c r="A16" s="37"/>
-      <c r="B16" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="C16" s="24"/>
+      <c r="A16" s="54"/>
+      <c r="B16" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16" s="15"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
     </row>
@@ -2521,7 +2510,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5877707E-8BDD-45A1-AE0E-C002F4BE2F0D}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0"/>
+    <sheetView topLeftCell="A8" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
@@ -2531,414 +2520,414 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="60.75" thickBot="1">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" s="26"/>
+      <c r="D1" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="39" t="s">
+    </row>
+    <row r="2" spans="1:5" ht="126.75" thickBot="1">
+      <c r="A2" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="39" t="s">
-        <v>74</v>
-      </c>
-      <c r="E1" s="39" t="s">
+      <c r="B2" s="28" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="126.75" thickBot="1">
-      <c r="A2" s="41" t="s">
+      <c r="C2" s="15"/>
+      <c r="D2" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="E2" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="42" t="s">
+    </row>
+    <row r="3" spans="1:5" ht="48" thickBot="1">
+      <c r="A3" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="E2" s="43" t="s">
+      <c r="B3" s="28" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="79.5" thickBot="1">
-      <c r="A3" s="41" t="s">
+      <c r="C3" s="15"/>
+      <c r="D3" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="B3" s="42" t="s">
+      <c r="E3" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="42" t="s">
+    </row>
+    <row r="4" spans="1:5" ht="95.25" thickBot="1">
+      <c r="A4" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="B4" s="28" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="126.75" thickBot="1">
-      <c r="A4" s="41" t="s">
+      <c r="C4" s="15"/>
+      <c r="D4" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="B4" s="42" t="s">
+      <c r="E4" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="42" t="s">
+    </row>
+    <row r="5" spans="1:5" ht="32.25" thickBot="1">
+      <c r="A5" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="E4" s="28" t="s">
+      <c r="B5" s="28" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="63.75" thickBot="1">
-      <c r="A5" s="41" t="s">
+      <c r="C5" s="15"/>
+      <c r="D5" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="B5" s="42" t="s">
+      <c r="E5" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="C5" s="24"/>
-      <c r="D5" s="42" t="s">
+    </row>
+    <row r="6" spans="1:5" ht="63.75" thickBot="1">
+      <c r="A6" s="30" t="s">
         <v>91</v>
       </c>
-      <c r="E5" s="42" t="s">
+      <c r="B6" s="28" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="63.75" thickBot="1">
-      <c r="A6" s="44" t="s">
+      <c r="C6" s="15"/>
+      <c r="D6" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="B6" s="42" t="s">
+      <c r="E6" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="42" t="s">
+    </row>
+    <row r="7" spans="1:5" ht="48" thickBot="1">
+      <c r="A7" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="E6" s="42" t="s">
+      <c r="B7" s="28" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="48" thickBot="1">
-      <c r="A7" s="41" t="s">
+      <c r="C7" s="15"/>
+      <c r="D7" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="B7" s="42" t="s">
+      <c r="E7" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="C7" s="24"/>
-      <c r="D7" s="42" t="s">
+    </row>
+    <row r="8" spans="1:5" ht="189.75" thickBot="1">
+      <c r="A8" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="E7" s="42" t="s">
+      <c r="B8" s="28" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="189.75" thickBot="1">
-      <c r="A8" s="44" t="s">
+      <c r="C8" s="28"/>
+      <c r="D8" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="E8" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42" t="s">
+    </row>
+    <row r="9" spans="1:5" ht="30" thickBot="1">
+      <c r="A9" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="E8" s="42" t="s">
+      <c r="B9" s="31" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="48" thickBot="1">
-      <c r="A9" s="41" t="s">
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="B9" s="45" t="s">
+    </row>
+    <row r="10" spans="1:5" ht="79.5" thickBot="1">
+      <c r="A10" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="42" t="s">
+      <c r="B10" s="28" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="79.5" thickBot="1">
-      <c r="A10" s="41" t="s">
+      <c r="C10" s="15"/>
+      <c r="D10" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="E10" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="C10" s="24"/>
-      <c r="D10" s="42" t="s">
+    </row>
+    <row r="11" spans="1:5" ht="79.5" thickBot="1">
+      <c r="A11" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="E10" s="42" t="s">
+      <c r="B11" s="28" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="79.5" thickBot="1">
-      <c r="A11" s="41" t="s">
+      <c r="C11" s="15"/>
+      <c r="D11" s="28" t="s">
         <v>112</v>
       </c>
-      <c r="B11" s="42" t="s">
+      <c r="E11" s="28" t="s">
         <v>113</v>
       </c>
-      <c r="C11" s="24"/>
-      <c r="D11" s="42" t="s">
+    </row>
+    <row r="12" spans="1:5" ht="111" thickBot="1">
+      <c r="A12" s="27" t="s">
         <v>114</v>
       </c>
-      <c r="E11" s="42" t="s">
+      <c r="B12" s="28" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="111" thickBot="1">
-      <c r="A12" s="41" t="s">
+      <c r="C12" s="15"/>
+      <c r="D12" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="B12" s="42" t="s">
+      <c r="E12" s="28" t="s">
         <v>117</v>
       </c>
-      <c r="C12" s="24"/>
-      <c r="D12" s="42" t="s">
+    </row>
+    <row r="13" spans="1:5" ht="79.5" thickBot="1">
+      <c r="A13" s="27" t="s">
         <v>118</v>
       </c>
-      <c r="E12" s="42" t="s">
+      <c r="B13" s="32" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="79.5" thickBot="1">
-      <c r="A13" s="41" t="s">
+      <c r="C13" s="15"/>
+      <c r="D13" s="28" t="s">
         <v>120</v>
       </c>
-      <c r="B13" s="46" t="s">
+      <c r="E13" s="28" t="s">
         <v>121</v>
       </c>
-      <c r="C13" s="24"/>
-      <c r="D13" s="42" t="s">
+    </row>
+    <row r="14" spans="1:5" ht="48" thickBot="1">
+      <c r="A14" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="E13" s="42" t="s">
+      <c r="B14" s="28" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="48" thickBot="1">
-      <c r="A14" s="41" t="s">
+      <c r="C14" s="15"/>
+      <c r="D14" s="28" t="s">
         <v>124</v>
       </c>
-      <c r="B14" s="42" t="s">
+      <c r="E14" s="28" t="s">
         <v>125</v>
       </c>
-      <c r="C14" s="24"/>
-      <c r="D14" s="42" t="s">
+    </row>
+    <row r="15" spans="1:5" ht="79.5" thickBot="1">
+      <c r="A15" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="E14" s="42" t="s">
+      <c r="B15" s="28" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="95.25" thickBot="1">
-      <c r="A15" s="41" t="s">
+      <c r="C15" s="15"/>
+      <c r="D15" s="28" t="s">
         <v>128</v>
       </c>
-      <c r="B15" s="42" t="s">
+      <c r="E15" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="C15" s="24"/>
-      <c r="D15" s="42" t="s">
+    </row>
+    <row r="16" spans="1:5" ht="63.75" thickBot="1">
+      <c r="A16" s="27" t="s">
         <v>130</v>
       </c>
-      <c r="E15" s="24" t="s">
+      <c r="B16" s="28" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="63.75" thickBot="1">
-      <c r="A16" s="41" t="s">
+      <c r="C16" s="15"/>
+      <c r="D16" s="28" t="s">
         <v>132</v>
       </c>
-      <c r="B16" s="42" t="s">
+      <c r="E16" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="C16" s="24"/>
-      <c r="D16" s="42" t="s">
+    </row>
+    <row r="17" spans="1:5" ht="63.75" thickBot="1">
+      <c r="A17" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="E16" s="42" t="s">
+      <c r="B17" s="28" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="63.75" thickBot="1">
-      <c r="A17" s="41" t="s">
+      <c r="C17" s="15"/>
+      <c r="D17" s="28" t="s">
         <v>136</v>
       </c>
-      <c r="B17" s="42" t="s">
+      <c r="E17" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="C17" s="24"/>
-      <c r="D17" s="42" t="s">
+    </row>
+    <row r="18" spans="1:5" ht="48" thickBot="1">
+      <c r="A18" s="27" t="s">
         <v>138</v>
       </c>
-      <c r="E17" s="42" t="s">
+      <c r="B18" s="28" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="48" thickBot="1">
-      <c r="A18" s="41" t="s">
+      <c r="C18" s="15"/>
+      <c r="D18" s="28" t="s">
         <v>140</v>
       </c>
-      <c r="B18" s="42" t="s">
+      <c r="E18" s="28" t="s">
         <v>141</v>
       </c>
-      <c r="C18" s="24"/>
-      <c r="D18" s="42" t="s">
+    </row>
+    <row r="19" spans="1:5" ht="63.75" thickBot="1">
+      <c r="A19" s="27" t="s">
         <v>142</v>
       </c>
-      <c r="E18" s="42" t="s">
+      <c r="B19" s="28" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="79.5" thickBot="1">
-      <c r="A19" s="41" t="s">
+      <c r="C19" s="15"/>
+      <c r="D19" s="28" t="s">
         <v>144</v>
       </c>
-      <c r="B19" s="42" t="s">
+      <c r="E19" s="28" t="s">
         <v>145</v>
       </c>
-      <c r="C19" s="24"/>
-      <c r="D19" s="42" t="s">
+    </row>
+    <row r="20" spans="1:5" ht="95.25" thickBot="1">
+      <c r="A20" s="27" t="s">
         <v>146</v>
       </c>
-      <c r="E19" s="42" t="s">
+      <c r="B20" s="33" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="95.25" thickBot="1">
-      <c r="A20" s="41" t="s">
+      <c r="C20" s="15"/>
+      <c r="D20" s="28" t="s">
         <v>148</v>
       </c>
-      <c r="B20" s="47" t="s">
+      <c r="E20" s="28" t="s">
         <v>149</v>
       </c>
-      <c r="C20" s="24"/>
-      <c r="D20" s="42" t="s">
+    </row>
+    <row r="21" spans="1:5" ht="63.75" thickBot="1">
+      <c r="A21" s="34" t="s">
         <v>150</v>
       </c>
-      <c r="E20" s="42" t="s">
+      <c r="B21" s="31" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="115.5" thickBot="1">
-      <c r="A21" s="48" t="s">
+      <c r="C21" s="15"/>
+      <c r="D21" s="28" t="s">
         <v>152</v>
       </c>
-      <c r="B21" s="45" t="s">
+      <c r="E21" s="28" t="s">
         <v>153</v>
       </c>
-      <c r="C21" s="24"/>
-      <c r="D21" s="42" t="s">
+    </row>
+    <row r="22" spans="1:5" ht="126.75" thickBot="1">
+      <c r="A22" s="35" t="s">
         <v>154</v>
       </c>
-      <c r="E21" s="42" t="s">
+      <c r="B22" s="36" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="126.75" thickBot="1">
-      <c r="A22" s="49" t="s">
+      <c r="C22" s="15"/>
+      <c r="D22" s="28" t="s">
         <v>156</v>
       </c>
-      <c r="B22" s="50" t="s">
+      <c r="E22" s="28" t="s">
         <v>157</v>
       </c>
-      <c r="C22" s="24"/>
-      <c r="D22" s="42" t="s">
+    </row>
+    <row r="23" spans="1:5" ht="61.5" thickBot="1">
+      <c r="A23" s="27" t="s">
         <v>158</v>
       </c>
-      <c r="E22" s="42" t="s">
+      <c r="B23" s="37" t="s">
+        <v>96</v>
+      </c>
+      <c r="C23" s="15"/>
+      <c r="D23" s="28" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="61.5" thickBot="1">
-      <c r="A23" s="41" t="s">
+      <c r="E23" s="28" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="79.5" thickBot="1">
+      <c r="A24" s="38" t="s">
         <v>160</v>
       </c>
-      <c r="B23" s="51" t="s">
-        <v>98</v>
-      </c>
-      <c r="C23" s="24"/>
-      <c r="D23" s="42" t="s">
+      <c r="B24" s="39" t="s">
         <v>161</v>
       </c>
-      <c r="E23" s="42" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="106.5" thickBot="1">
-      <c r="A24" s="52" t="s">
+      <c r="C24" s="15"/>
+      <c r="D24" s="28" t="s">
         <v>162</v>
       </c>
-      <c r="B24" s="53" t="s">
+      <c r="E24" s="28" t="s">
         <v>163</v>
       </c>
-      <c r="C24" s="24"/>
-      <c r="D24" s="42" t="s">
+    </row>
+    <row r="25" spans="1:5" ht="106.5" thickBot="1">
+      <c r="A25" s="27" t="s">
         <v>164</v>
       </c>
-      <c r="E24" s="42" t="s">
+      <c r="B25" s="29" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="126.75" thickBot="1">
-      <c r="A25" s="41" t="s">
+      <c r="C25" s="15"/>
+      <c r="D25" s="28" t="s">
         <v>166</v>
       </c>
-      <c r="B25" s="43" t="s">
+      <c r="E25" s="28" t="s">
         <v>167</v>
       </c>
-      <c r="C25" s="24"/>
-      <c r="D25" s="42" t="s">
+    </row>
+    <row r="26" spans="1:5" ht="63.75" thickBot="1">
+      <c r="A26" s="17"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="28" t="s">
         <v>168</v>
       </c>
-      <c r="E25" s="42" t="s">
+      <c r="E26" s="29" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="63.75" thickBot="1">
-      <c r="A26" s="26"/>
-      <c r="B26" s="24"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="42" t="s">
+    <row r="27" spans="1:5" ht="409.6" thickBot="1">
+      <c r="A27" s="30" t="s">
         <v>170</v>
       </c>
-      <c r="E26" s="43" t="s">
+      <c r="B27" s="28" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" ht="409.6" thickBot="1">
-      <c r="A27" s="44" t="s">
+      <c r="C27" s="15"/>
+      <c r="D27" s="28" t="s">
         <v>172</v>
       </c>
-      <c r="B27" s="42" t="s">
+      <c r="E27" s="40" t="s">
         <v>173</v>
       </c>
-      <c r="C27" s="24"/>
-      <c r="D27" s="42" t="s">
+    </row>
+    <row r="28" spans="1:5" ht="32.25" thickBot="1">
+      <c r="A28" s="27" t="s">
         <v>174</v>
       </c>
-      <c r="E27" s="54" t="s">
+      <c r="B28" s="31" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" ht="79.5" thickBot="1">
-      <c r="A28" s="41" t="s">
-        <v>176</v>
-      </c>
-      <c r="B28" s="45" t="s">
-        <v>177</v>
-      </c>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2946,4 +2935,18 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDCA4992-5691-4FD5-A5D6-6D45452CCE7D}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>